<commit_message>
Backend first complete draft
</commit_message>
<xml_diff>
--- a/uploadedFiles/testData.xlsx
+++ b/uploadedFiles/testData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Matric</t>
   </si>
@@ -52,6 +52,18 @@
   </si>
   <si>
     <t>awojirin@gmail.com</t>
+  </si>
+  <si>
+    <t>Omoniyi</t>
+  </si>
+  <si>
+    <t>omoniyi@gmail.com</t>
+  </si>
+  <si>
+    <t>adult edu</t>
+  </si>
+  <si>
+    <t>eiueh485</t>
   </si>
 </sst>
 </file>
@@ -380,10 +392,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -451,10 +463,31 @@
         <v>23448</v>
       </c>
     </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>206068</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4">
+        <v>300</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
     <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="C4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed config so you don't have to fix anything
</commit_message>
<xml_diff>
--- a/uploadedFiles/testData.xlsx
+++ b/uploadedFiles/testData.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14A17B44-F0C1-4029-A326-145E72B28A9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="5055" yWindow="4245" windowWidth="9840" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>Matric</t>
   </si>
@@ -64,12 +65,21 @@
   </si>
   <si>
     <t>eiueh485</t>
+  </si>
+  <si>
+    <t>Adelola John</t>
+  </si>
+  <si>
+    <t>adelolajohn@gmail.com</t>
+  </si>
+  <si>
+    <t>Civil Eng.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -391,11 +401,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -483,11 +493,32 @@
         <v>14</v>
       </c>
     </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>200977</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5">
+        <v>300</v>
+      </c>
+      <c r="F5">
+        <v>564473</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{A96A8FB9-F9F1-4375-8504-C0D36A1AC248}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>